<commit_message>
Update example input files to newest format, add Data-input files
</commit_message>
<xml_diff>
--- a/data/example/Power_Demand.xlsx
+++ b/data/example/Power_Demand.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ScenarioA" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="ScenarioA" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -629,7 +629,7 @@
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t>v0.1.2</t>
+          <t>v0.1.3</t>
         </is>
       </c>
     </row>
@@ -1157,122 +1157,122 @@
       </c>
       <c r="G7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="H7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="I7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="J7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="K7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="L7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="M7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="N7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="O7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="P7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="Q7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="R7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="S7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="T7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="U7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="V7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="W7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="X7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="Y7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="Z7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="AA7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="AB7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="AC7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="AD7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update data/example files to newest versions and update comparison .mps
</commit_message>
<xml_diff>
--- a/data/example/Power_Demand.xlsx
+++ b/data/example/Power_Demand.xlsx
@@ -629,7 +629,7 @@
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t>v0.1.3</t>
+          <t>v0.1.4</t>
         </is>
       </c>
     </row>
@@ -955,7 +955,7 @@
       </c>
       <c r="G5" s="8" t="inlineStr">
         <is>
-          <t>Demand at node for representative hour k</t>
+          <t>Demand at this representative time step k</t>
         </is>
       </c>
       <c r="H5" s="7" t="n"/>

</xml_diff>